<commit_message>
updated code and team report file
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18980" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="180">
   <si>
     <t>Initials</t>
   </si>
@@ -763,11 +763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1963887632"/>
-        <c:axId val="1963889952"/>
+        <c:axId val="-796605504"/>
+        <c:axId val="-795704528"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1963887632"/>
+        <c:axId val="-796605504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -787,14 +787,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963889952"/>
+        <c:crossAx val="-795704528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1963889952"/>
+        <c:axId val="-795704528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963887632"/>
+        <c:crossAx val="-796605504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8256,8 +8256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8373,7 +8373,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8390,7 +8390,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -23663,7 +23663,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23805,9 +23805,15 @@
       <c r="F6" s="2">
         <v>35</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="2">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2">
+        <v>45</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
@@ -23825,9 +23831,15 @@
       <c r="F7" s="2">
         <v>30</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="2">
+        <v>30</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
@@ -37342,7 +37354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated team report file
updated team report file
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="179">
   <si>
     <t>Initials</t>
   </si>
@@ -645,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,6 +675,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -765,11 +766,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="311283904"/>
-        <c:axId val="275839168"/>
+        <c:axId val="-1550644416"/>
+        <c:axId val="-1550642096"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="311283904"/>
+        <c:axId val="-1550644416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -789,14 +790,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275839168"/>
+        <c:crossAx val="-1550642096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="275839168"/>
+        <c:axId val="-1550642096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +831,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311283904"/>
+        <c:crossAx val="-1550644416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8258,8 +8259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="B25" sqref="B18:D25"/>
+    <sheetView zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8519,7 +8520,9 @@
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
@@ -8534,7 +8537,9 @@
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
@@ -8549,7 +8554,9 @@
       <c r="D16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
@@ -8564,7 +8571,9 @@
       <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
@@ -33852,8 +33861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -33970,11 +33979,20 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D6" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6">
         <v>40</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -33987,11 +34005,20 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E7">
         <v>15</v>
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7">
+        <v>28</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -34004,6 +34031,9 @@
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="D8" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E8">
         <v>10</v>
       </c>
@@ -34020,6 +34050,9 @@
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>177</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -35028,7 +35061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed user stories for sprint 3
updated team report file
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="181">
   <si>
     <t>Initials</t>
   </si>
@@ -782,11 +782,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1450774880"/>
-        <c:axId val="-1450772560"/>
+        <c:axId val="374290992"/>
+        <c:axId val="374293312"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1450774880"/>
+        <c:axId val="374290992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,14 +806,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1450772560"/>
+        <c:crossAx val="374293312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1450772560"/>
+        <c:axId val="374293312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,7 +847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1450774880"/>
+        <c:crossAx val="374290992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8276,7 +8276,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8672,7 +8672,9 @@
       <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
@@ -8687,7 +8689,9 @@
       <c r="D23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
@@ -15621,14 +15625,14 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" customWidth="1"/>
     <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
@@ -23697,7 +23701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -33910,7 +33914,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScale="187" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35209,8 +35213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="192" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -35327,11 +35331,17 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D6" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6">
         <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -35344,11 +35354,23 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <v>20</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -36386,7 +36408,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C9"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -37561,8 +37583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="215" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
updated burn down chart in team report
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -797,11 +797,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1157954912"/>
-        <c:axId val="1157957232"/>
+        <c:axId val="-1091479440"/>
+        <c:axId val="-1006601776"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1157954912"/>
+        <c:axId val="-1091479440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,14 +821,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1157957232"/>
+        <c:crossAx val="-1006601776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1157957232"/>
+        <c:axId val="-1006601776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1157954912"/>
+        <c:crossAx val="-1091479440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8290,8 +8290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15651,8 +15651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15765,7 +15765,10 @@
         <f>SUM(Sprint3!H2:H9)</f>
         <v>200</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6">
+        <f>(D4-D3)/E4*60</f>
+        <v>-96.9</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>

</xml_diff>

<commit_message>
completed sprint 4 user stories
updated team report file and completed sprint 4 user stories
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="185">
   <si>
     <t>Initials</t>
   </si>
@@ -587,6 +587,9 @@
   <si>
     <t>Coming late for meetings</t>
   </si>
+  <si>
+    <t>Yes</t>
+  </si>
 </sst>
 </file>
 
@@ -596,7 +599,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -638,6 +641,12 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -662,9 +671,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -702,7 +712,8 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -760,6 +771,9 @@
                 <c:pt idx="2">
                   <c:v>42674.0</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>42689.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -777,6 +791,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,11 +814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1091479440"/>
-        <c:axId val="-1006601776"/>
+        <c:axId val="1092657584"/>
+        <c:axId val="1092659632"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1091479440"/>
+        <c:axId val="1092657584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,14 +838,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1006601776"/>
+        <c:crossAx val="1092659632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1006601776"/>
+        <c:axId val="1092659632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1091479440"/>
+        <c:crossAx val="1092657584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,7 +1202,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8290,8 +8307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A9" zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8823,7 +8840,9 @@
       <c r="D30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
@@ -8838,7 +8857,9 @@
       <c r="D31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
@@ -15651,8 +15672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15771,12 +15792,27 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="6"/>
+      <c r="A5" s="5">
+        <v>42689</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <f>SUM(Sprint4!G2:G9)</f>
+        <v>32</v>
+      </c>
+      <c r="E5" s="2">
+        <f>SUM(Sprint4!H2:H9)</f>
+        <v>35</v>
+      </c>
+      <c r="F5" s="6">
+        <f>(D5-D4)/E5*60</f>
+        <v>-229.71428571428572</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5"/>
@@ -36560,8 +36596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView zoomScale="168" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -36678,11 +36714,23 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D6" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6">
         <v>25</v>
+      </c>
+      <c r="G6">
+        <v>29</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -36695,11 +36743,23 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="E7">
         <v>20</v>
       </c>
       <c r="F7">
         <v>30</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -36712,6 +36772,7 @@
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="D8" s="17"/>
       <c r="E8">
         <v>30</v>
       </c>
@@ -37736,8 +37797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="215" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A11" zoomScale="215" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -42074,5 +42135,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated team report and user stories
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18660" activeTab="6"/>
+    <workbookView xWindow="18740" yWindow="440" windowWidth="14860" windowHeight="18660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="188">
   <si>
     <t>Initials</t>
   </si>
@@ -593,6 +593,12 @@
   <si>
     <t>psingh5712</t>
   </si>
+  <si>
+    <t>Waiting till last day to complete user story.</t>
+  </si>
+  <si>
+    <t>Work user story individually at your own place.</t>
+  </si>
 </sst>
 </file>
 
@@ -817,11 +823,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1482915888"/>
-        <c:axId val="-1483520672"/>
+        <c:axId val="492481728"/>
+        <c:axId val="492484048"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1482915888"/>
+        <c:axId val="492481728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -841,14 +847,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1483520672"/>
+        <c:crossAx val="492484048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1483520672"/>
+        <c:axId val="492484048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1482915888"/>
+        <c:crossAx val="492481728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8310,8 +8316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="182" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8783,7 +8789,9 @@
       <c r="D26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
@@ -8798,7 +8806,9 @@
       <c r="D27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
@@ -15683,7 +15693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -15814,15 +15824,15 @@
       </c>
       <c r="D5" s="2">
         <f>SUM(Sprint4!G2:G9)</f>
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="E5" s="2">
         <f>SUM(Sprint4!H2:H9)</f>
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="F5" s="6">
         <f>(D5-D4)/E5*60</f>
-        <v>-19.862068965517242</v>
+        <v>-4.8648648648648649</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -35308,7 +35318,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -36607,14 +36617,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="179" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -36657,11 +36667,23 @@
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D2" s="17" t="s">
+        <v>176</v>
+      </c>
       <c r="E2">
         <v>25</v>
       </c>
       <c r="F2">
         <v>40</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -36674,11 +36696,23 @@
       <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D3" s="17" t="s">
+        <v>176</v>
+      </c>
       <c r="E3">
         <v>25</v>
       </c>
       <c r="F3">
         <v>35</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -36860,24 +36894,50 @@
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -37855,8 +37915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="215" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>